<commit_message>
newVolumetric report & store list
</commit_message>
<xml_diff>
--- a/backend/src/scripts/RAPORT BAZY.xlsx
+++ b/backend/src/scripts/RAPORT BAZY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bartlomiej.babula\Desktop\eSambo SELENIUM\eSambo_helpdesk\helpdesk_app\backend\src\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F82D7E6-52D3-4467-AA07-59AC01DA3613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D182A3-408D-4F00-862D-E0FF9DD58117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Obliczenia" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>Przed ostatni wpis w raporcie – na ile sklepów wystarczy…</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>WS2</t>
-  </si>
-  <si>
-    <t>WS3</t>
-  </si>
-  <si>
-    <t>WS4</t>
   </si>
   <si>
     <t>Średnie obciążenie</t>
@@ -321,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -360,9 +354,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thin">
         <color indexed="8"/>
       </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="hair">
         <color indexed="8"/>
       </right>
@@ -373,9 +378,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="hair">
         <color indexed="8"/>
       </right>
@@ -384,9 +387,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
+      <left/>
       <right style="hair">
         <color indexed="8"/>
       </right>
@@ -403,9 +404,11 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -416,7 +419,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -424,6 +427,36 @@
       <left/>
       <right style="thin">
         <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -437,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -447,14 +480,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -477,9 +505,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -496,15 +521,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -869,212 +914,6 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Obliczenia!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>WS3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="FFFF00"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Obliczenia!$A$5:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>d/mm/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>44533</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44534</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44535</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44536</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44537</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44538</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44539</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Obliczenia!$D$5:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-20A1-433B-B312-1242815B1026}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Obliczenia!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>WS4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="00FFFF"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="00FFFF"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Obliczenia!$A$5:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>d/mm/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>44533</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44534</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>44535</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44536</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>44537</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>44538</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44539</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Obliczenia!$E$5:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-20A1-433B-B312-1242815B1026}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
@@ -1188,6 +1027,208 @@
         <c:smooth val="0"/>
         <c:axId val="1548149743"/>
         <c:axId val="1"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$D$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="12700">
+                    <a:solidFill>
+                      <a:srgbClr val="FFFF00"/>
+                    </a:solidFill>
+                    <a:prstDash val="solid"/>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:srgbClr val="FFFF00"/>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="FFFF00"/>
+                      </a:solidFill>
+                      <a:prstDash val="solid"/>
+                    </a:ln>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$A$5:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>d/mm/yyyy</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>44533</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>44534</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44535</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44537</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44538</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44539</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$D$5:$D$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-20A1-433B-B312-1242815B1026}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$E$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="12700">
+                    <a:solidFill>
+                      <a:srgbClr val="00FFFF"/>
+                    </a:solidFill>
+                    <a:prstDash val="solid"/>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="x"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:solidFill>
+                        <a:srgbClr val="00FFFF"/>
+                      </a:solidFill>
+                      <a:prstDash val="solid"/>
+                    </a:ln>
+                  </c:spPr>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$A$5:$A$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>d/mm/yyyy</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>44533</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>44534</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>44535</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>44536</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>44537</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>44538</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>44539</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Obliczenia!$E$5:$E$11</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-20A1-433B-B312-1242815B1026}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:dateAx>
         <c:axId val="1548149743"/>
@@ -2245,8 +2286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2276,209 +2317,177 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="4">
         <v>990</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="8">
         <f>90/F14</f>
         <v>4628.5714285714294</v>
       </c>
-      <c r="H3" s="11">
-        <f>G3/4</f>
-        <v>1157.1428571428573</v>
+      <c r="H3" s="8">
+        <f>G3/2</f>
+        <v>2314.2857142857147</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="19" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>44533</v>
+      </c>
+      <c r="B5" s="16">
+        <v>24</v>
+      </c>
+      <c r="C5" s="36">
+        <v>37</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="27">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>44534</v>
+      </c>
+      <c r="B6" s="16">
+        <v>21</v>
+      </c>
+      <c r="C6" s="36">
+        <v>33</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="27">
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>44535</v>
+      </c>
+      <c r="B7" s="16">
+        <v>18</v>
+      </c>
+      <c r="C7" s="36">
+        <v>29</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="27">
+        <v>22.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>44536</v>
+      </c>
+      <c r="B8" s="16">
+        <v>15</v>
+      </c>
+      <c r="C8" s="36">
+        <v>25</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="27">
+        <v>19.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>44537</v>
+      </c>
+      <c r="B9" s="16">
+        <v>12</v>
+      </c>
+      <c r="C9" s="36">
+        <v>21</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="27">
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>44538</v>
+      </c>
+      <c r="B10" s="16">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>44533</v>
-      </c>
-      <c r="B5" s="20">
-        <v>24</v>
-      </c>
-      <c r="C5" s="20">
-        <v>37</v>
-      </c>
-      <c r="D5" s="20">
-        <v>27</v>
-      </c>
-      <c r="E5" s="20">
-        <v>31</v>
-      </c>
-      <c r="F5" s="7">
-        <v>29.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>44534</v>
-      </c>
-      <c r="B6" s="20">
-        <v>21</v>
-      </c>
-      <c r="C6" s="20">
-        <v>33</v>
-      </c>
-      <c r="D6" s="20">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20">
-        <v>27</v>
-      </c>
-      <c r="F6" s="7">
-        <v>26.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>44535</v>
-      </c>
-      <c r="B7" s="20">
-        <v>18</v>
-      </c>
-      <c r="C7" s="20">
-        <v>29</v>
-      </c>
-      <c r="D7" s="20">
-        <v>21</v>
-      </c>
-      <c r="E7" s="20">
-        <v>23</v>
-      </c>
-      <c r="F7" s="7">
-        <v>22.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>44536</v>
-      </c>
-      <c r="B8" s="20">
-        <v>15</v>
-      </c>
-      <c r="C8" s="20">
-        <v>25</v>
-      </c>
-      <c r="D8" s="20">
-        <v>18</v>
-      </c>
-      <c r="E8" s="20">
-        <v>19</v>
-      </c>
-      <c r="F8" s="7">
-        <v>19.25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>44537</v>
-      </c>
-      <c r="B9" s="20">
-        <v>12</v>
-      </c>
-      <c r="C9" s="20">
-        <v>21</v>
-      </c>
-      <c r="D9" s="20">
-        <v>15</v>
-      </c>
-      <c r="E9" s="20">
-        <v>15</v>
-      </c>
-      <c r="F9" s="7">
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>44538</v>
-      </c>
-      <c r="B10" s="20">
-        <v>9</v>
-      </c>
-      <c r="C10" s="20">
+      <c r="C10" s="36">
         <v>17</v>
       </c>
-      <c r="D10" s="20">
-        <v>12</v>
-      </c>
-      <c r="E10" s="20">
-        <v>11</v>
-      </c>
-      <c r="F10" s="7">
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="27">
         <v>12.25</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>44539</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="16">
         <v>6</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="36">
         <v>13</v>
       </c>
-      <c r="D11" s="20">
-        <v>9</v>
-      </c>
-      <c r="E11" s="20">
-        <v>7</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="28">
         <v>8.75</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="21"/>
-      <c r="F13" s="23">
+      <c r="D13" s="17"/>
+      <c r="F13" s="19">
         <v>19.25</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="23">
+      <c r="F14" s="19">
         <v>1.9444444444444441E-2</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E15" s="22"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>14623.380859375</v>
@@ -2486,7 +2495,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>14099.7998046875</v>
@@ -2494,7 +2503,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>523.5810546875</v>
@@ -2502,7 +2511,7 @@
     </row>
     <row r="19" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <f>Tabela!J17</f>
@@ -2510,10 +2519,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="23">
+      <c r="A20" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="19">
         <f>B18/B19</f>
         <v>55.607736898167211</v>
       </c>
@@ -2530,112 +2539,112 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>18</v>
+      <c r="A29" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B29">
         <v>13100.77221679688</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>19</v>
+      <c r="A30" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B30">
         <v>13113.44488525391</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>20</v>
+      <c r="A31" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="B31">
         <v>13120.892944335939</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
-        <v>21</v>
+      <c r="A32" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B32">
         <v>13125.213684082029</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
-        <v>22</v>
+      <c r="A33" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="B33">
         <v>13133.80029296875</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="15" t="s">
-        <v>23</v>
+      <c r="A34" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B34">
         <v>13141.6015625</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
-        <v>24</v>
+      <c r="A35" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B35">
         <v>13159.392761230471</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
-        <v>25</v>
+      <c r="A36" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="B36">
         <v>13170.230163574221</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>26</v>
+      <c r="A37" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="B37">
         <v>13178.9443359375</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
-        <v>27</v>
+      <c r="A38" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="B38">
         <v>13186.893432617189</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>28</v>
+      <c r="A39" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="B39">
         <v>13190.53668212891</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
-        <v>29</v>
+      <c r="A40" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="B40">
         <v>13199.576049804689</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
-        <v>30</v>
+      <c r="A41" s="12" t="s">
+        <v>28</v>
       </c>
       <c r="B41">
         <v>13208.655578613279</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="15" t="s">
-        <v>31</v>
+      <c r="A42" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B42">
         <v>13218.460571289061</v>
@@ -2670,7 +2679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2690,325 +2699,325 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="24"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="4" spans="4:12" ht="63.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="I4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="9" t="s">
+    </row>
+    <row r="5" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="E5" s="21">
+        <v>1366.96</v>
+      </c>
+      <c r="F5" s="21">
+        <v>1389.9</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1678.29</v>
+      </c>
+      <c r="H5" s="21">
+        <v>1.8</v>
+      </c>
+      <c r="I5" s="21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="10" t="s">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="25">
-        <v>1366.96</v>
-      </c>
-      <c r="F5" s="25">
-        <v>1389.9</v>
-      </c>
-      <c r="G5" s="25">
-        <v>1678.29</v>
-      </c>
-      <c r="H5" s="25">
-        <v>1.8</v>
-      </c>
-      <c r="I5" s="25" t="s">
+      <c r="E6" s="21">
+        <v>153.02000000000001</v>
+      </c>
+      <c r="F6" s="21">
+        <v>153.63999999999999</v>
+      </c>
+      <c r="G6" s="21">
+        <v>45.79</v>
+      </c>
+      <c r="H6" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="10" t="s">
+      <c r="E7" s="21">
+        <v>2466.25</v>
+      </c>
+      <c r="F7" s="21">
+        <v>2489.0300000000002</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1666.25</v>
+      </c>
+      <c r="H7" s="21">
+        <v>1.79</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="4:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="25">
-        <v>153.02000000000001</v>
-      </c>
-      <c r="F6" s="25">
-        <v>153.63999999999999</v>
-      </c>
-      <c r="G6" s="25">
-        <v>45.79</v>
-      </c>
-      <c r="H6" s="25">
-        <v>0.05</v>
-      </c>
-      <c r="I6" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="10" t="s">
+      <c r="E8" s="21">
+        <v>957.49</v>
+      </c>
+      <c r="F8" s="21">
+        <v>969.25</v>
+      </c>
+      <c r="G8" s="21">
+        <v>860.43</v>
+      </c>
+      <c r="H8" s="21">
+        <v>0.92</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="4:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="25">
-        <v>2466.25</v>
-      </c>
-      <c r="F7" s="25">
-        <v>2489.0300000000002</v>
-      </c>
-      <c r="G7" s="25">
-        <v>1666.25</v>
-      </c>
-      <c r="H7" s="25">
-        <v>1.79</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="4:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="10" t="s">
+      <c r="E9" s="21">
+        <v>103.18</v>
+      </c>
+      <c r="F9" s="21">
+        <v>103.18</v>
+      </c>
+      <c r="G9" s="21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="25">
-        <v>957.49</v>
-      </c>
-      <c r="F8" s="25">
-        <v>969.25</v>
-      </c>
-      <c r="G8" s="25">
-        <v>860.43</v>
-      </c>
-      <c r="H8" s="25">
-        <v>0.92</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="4:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="10" t="s">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="4:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="25">
-        <v>103.18</v>
-      </c>
-      <c r="F9" s="25">
-        <v>103.18</v>
-      </c>
-      <c r="G9" s="25">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="H9" s="25">
+      <c r="E10" s="21">
+        <v>185.3</v>
+      </c>
+      <c r="F10" s="21">
+        <v>187.27</v>
+      </c>
+      <c r="G10" s="21">
+        <v>143.88</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="4:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="21">
+        <v>500.79</v>
+      </c>
+      <c r="F11" s="21">
+        <v>495.59</v>
+      </c>
+      <c r="G11" s="21">
         <v>0</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="4:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="10" t="s">
+      <c r="H11" s="21">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="4:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="25">
-        <v>185.3</v>
-      </c>
-      <c r="F10" s="25">
-        <v>187.27</v>
-      </c>
-      <c r="G10" s="25">
-        <v>143.88</v>
-      </c>
-      <c r="H10" s="25">
-        <v>0.15</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="4:12" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="10" t="s">
+      <c r="E12" s="21">
+        <v>557</v>
+      </c>
+      <c r="F12" s="21">
+        <v>561.41999999999996</v>
+      </c>
+      <c r="G12" s="21">
+        <v>323</v>
+      </c>
+      <c r="H12" s="21">
+        <v>0.35</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="25">
-        <v>500.79</v>
-      </c>
-      <c r="F11" s="25">
-        <v>495.59</v>
-      </c>
-      <c r="G11" s="25">
-        <v>0</v>
-      </c>
-      <c r="H11" s="25">
-        <v>0</v>
-      </c>
-      <c r="I11" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="4:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="10" t="s">
+      <c r="E13" s="21">
+        <v>768.69</v>
+      </c>
+      <c r="F13" s="21">
+        <v>773.92</v>
+      </c>
+      <c r="G13" s="21">
+        <v>382.79</v>
+      </c>
+      <c r="H13" s="21">
+        <v>0.41</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="25">
-        <v>557</v>
-      </c>
-      <c r="F12" s="25">
-        <v>561.41999999999996</v>
-      </c>
-      <c r="G12" s="25">
-        <v>323</v>
-      </c>
-      <c r="H12" s="25">
-        <v>0.35</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="10" t="s">
+      <c r="E14" s="21">
+        <v>59.44</v>
+      </c>
+      <c r="F14" s="21">
+        <v>59.76</v>
+      </c>
+      <c r="G14" s="21">
+        <v>23.43</v>
+      </c>
+      <c r="H14" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="25">
-        <v>768.69</v>
-      </c>
-      <c r="F13" s="25">
-        <v>773.92</v>
-      </c>
-      <c r="G13" s="25">
-        <v>382.79</v>
-      </c>
-      <c r="H13" s="25">
-        <v>0.41</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="10" t="s">
+      <c r="E15" s="21">
+        <v>732.49</v>
+      </c>
+      <c r="F15" s="21">
+        <v>737.51</v>
+      </c>
+      <c r="G15" s="21">
+        <v>367.02</v>
+      </c>
+      <c r="H15" s="21">
+        <v>0.39</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="25">
-        <v>59.44</v>
-      </c>
-      <c r="F14" s="25">
-        <v>59.76</v>
-      </c>
-      <c r="G14" s="25">
-        <v>23.43</v>
-      </c>
-      <c r="H14" s="25">
-        <v>0.03</v>
-      </c>
-      <c r="I14" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="10" t="s">
+      <c r="E16" s="21">
+        <v>1488.49</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1545.23</v>
+      </c>
+      <c r="G16" s="21">
+        <v>4150.6400000000003</v>
+      </c>
+      <c r="H16" s="21">
+        <v>4.45</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="25">
-        <v>732.49</v>
-      </c>
-      <c r="F15" s="25">
-        <v>737.51</v>
-      </c>
-      <c r="G15" s="25">
-        <v>367.02</v>
-      </c>
-      <c r="H15" s="25">
-        <v>0.39</v>
-      </c>
-      <c r="I15" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="4:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="10" t="s">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="25">
-        <v>1488.49</v>
-      </c>
-      <c r="F16" s="25">
-        <v>1545.23</v>
-      </c>
-      <c r="G16" s="25">
-        <v>4150.6400000000003</v>
-      </c>
-      <c r="H16" s="25">
-        <v>4.45</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="26">
+      <c r="E17" s="22">
         <f>SUM(E5:E16)</f>
         <v>9339.1</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="22">
         <f>SUM(F5:F16)</f>
         <v>9465.7000000000007</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="22">
         <f>SUM(G5:G16)</f>
         <v>9641.59</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="22">
         <f>SUM(H5:H16)</f>
         <v>10.34</v>
       </c>
-      <c r="I17" s="27"/>
-      <c r="J17" s="14">
+      <c r="I17" s="23"/>
+      <c r="J17" s="11">
         <f>G17/1024</f>
         <v>9.4156152343750001</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>